<commit_message>
Add remote content (#140)
* Add remote content

* Add remote content
</commit_message>
<xml_diff>
--- a/examples/minimal/reporting engine input/ObservedData/Itraconazole 600mg MD.xlsx
+++ b/examples/minimal/reporting engine input/ObservedData/Itraconazole 600mg MD.xlsx
@@ -19,10 +19,10 @@
     <t>Time  [h]</t>
   </si>
   <si>
-    <t>SD  [mg/l]</t>
+    <t>Conc  [mg/l]</t>
   </si>
   <si>
-    <t>Conc  [mg/l]</t>
+    <t>SD  [mg/l]</t>
   </si>
 </sst>
 </file>
@@ -142,10 +142,10 @@
         <v>73</v>
       </c>
       <c r="B2" s="15">
+        <v>10.660510063171387</v>
+      </c>
+      <c r="C2" s="15">
         <v>4.7607641220092773</v>
-      </c>
-      <c r="C2" s="15">
-        <v>10.660510063171387</v>
       </c>
     </row>
     <row r="3">
@@ -153,10 +153,10 @@
         <v>74</v>
       </c>
       <c r="B3" s="15">
+        <v>9.60813045501709</v>
+      </c>
+      <c r="C3" s="15">
         <v>3.0621869564056396</v>
-      </c>
-      <c r="C3" s="15">
-        <v>9.60813045501709</v>
       </c>
     </row>
     <row r="4">
@@ -164,10 +164,10 @@
         <v>75</v>
       </c>
       <c r="B4" s="15">
+        <v>7.9942512512207031</v>
+      </c>
+      <c r="C4" s="15">
         <v>2.2343277931213379</v>
-      </c>
-      <c r="C4" s="15">
-        <v>7.9942512512207031</v>
       </c>
     </row>
     <row r="5">
@@ -175,10 +175,10 @@
         <v>76</v>
       </c>
       <c r="B5" s="15">
+        <v>6.7048468589782715</v>
+      </c>
+      <c r="C5" s="15">
         <v>1.9884419441223145</v>
-      </c>
-      <c r="C5" s="15">
-        <v>6.7048468589782715</v>
       </c>
     </row>
     <row r="6">
@@ -186,10 +186,10 @@
         <v>78</v>
       </c>
       <c r="B6" s="15">
+        <v>3.9241900444030762</v>
+      </c>
+      <c r="C6" s="15">
         <v>1.314033031463623</v>
-      </c>
-      <c r="C6" s="15">
-        <v>3.9241900444030762</v>
       </c>
     </row>
     <row r="7">
@@ -197,10 +197,10 @@
         <v>80</v>
       </c>
       <c r="B7" s="15">
+        <v>2.5482971668243408</v>
+      </c>
+      <c r="C7" s="15">
         <v>1.3559880256652832</v>
-      </c>
-      <c r="C7" s="15">
-        <v>2.5482971668243408</v>
       </c>
     </row>
     <row r="8">
@@ -208,10 +208,10 @@
         <v>145</v>
       </c>
       <c r="B8" s="15">
+        <v>7.6198148727416992</v>
+      </c>
+      <c r="C8" s="15">
         <v>4.5570683479309082</v>
-      </c>
-      <c r="C8" s="15">
-        <v>7.6198148727416992</v>
       </c>
     </row>
     <row r="9">
@@ -219,10 +219,10 @@
         <v>146</v>
       </c>
       <c r="B9" s="15">
+        <v>9.0128288269042969</v>
+      </c>
+      <c r="C9" s="15">
         <v>2.6220240592956543</v>
-      </c>
-      <c r="C9" s="15">
-        <v>9.0128288269042969</v>
       </c>
     </row>
     <row r="10">
@@ -230,10 +230,10 @@
         <v>147</v>
       </c>
       <c r="B10" s="15">
+        <v>6.9227356910705566</v>
+      </c>
+      <c r="C10" s="15">
         <v>2.3181090354919434</v>
-      </c>
-      <c r="C10" s="15">
-        <v>6.9227356910705566</v>
       </c>
     </row>
     <row r="11">
@@ -241,10 +241,10 @@
         <v>148</v>
       </c>
       <c r="B11" s="15">
+        <v>5.6234130859375</v>
+      </c>
+      <c r="C11" s="15">
         <v>1.883025050163269</v>
-      </c>
-      <c r="C11" s="15">
-        <v>5.6234130859375</v>
       </c>
     </row>
     <row r="12">
@@ -252,10 +252,10 @@
         <v>150</v>
       </c>
       <c r="B12" s="15">
+        <v>2.850106954574585</v>
+      </c>
+      <c r="C12" s="15">
         <v>1.2473740577697754</v>
-      </c>
-      <c r="C12" s="15">
-        <v>2.850106954574585</v>
       </c>
     </row>
     <row r="13">
@@ -263,10 +263,10 @@
         <v>152</v>
       </c>
       <c r="B13" s="15">
+        <v>1.7223089933395386</v>
+      </c>
+      <c r="C13" s="15">
         <v>1.2468825578689575</v>
-      </c>
-      <c r="C13" s="15">
-        <v>1.7223089933395386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>